<commit_message>
Part1: Expected 3 outputs
</commit_message>
<xml_diff>
--- a/data/Sample_input_abstracts.xlsx
+++ b/data/Sample_input_abstracts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="297">
   <si>
     <t>Poster #</t>
   </si>
@@ -683,6 +683,231 @@
   <si>
     <t>Reed</t>
   </si>
+  <si>
+    <t>AI in Mental Health Diagnosis</t>
+  </si>
+  <si>
+    <t>Using machine learning to detect mental health conditions.</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Foster</t>
+  </si>
+  <si>
+    <t>Psychology &amp; AI</t>
+  </si>
+  <si>
+    <t>Smart Prosthetics and Bionics</t>
+  </si>
+  <si>
+    <t>AI-powered prosthetics improving mobility.</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>Barnes</t>
+  </si>
+  <si>
+    <t>The Future of Electric Aircraft</t>
+  </si>
+  <si>
+    <t>Advancements in battery tech for aviation.</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Henderson</t>
+  </si>
+  <si>
+    <t>AI-Powered Smart Homes</t>
+  </si>
+  <si>
+    <t>Enhancing home automation with artificial intelligence.</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Bailey</t>
+  </si>
+  <si>
+    <t>The Role of AI in Criminal Justice</t>
+  </si>
+  <si>
+    <t>Examining AI’s impact on legal decision-making.</t>
+  </si>
+  <si>
+    <t>Elijah</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>Sustainable Space Exploration</t>
+  </si>
+  <si>
+    <t>Using renewable tech for deep space missions.</t>
+  </si>
+  <si>
+    <t>Abigail</t>
+  </si>
+  <si>
+    <t>Rivera</t>
+  </si>
+  <si>
+    <t>AI in Sports Performance Analysis</t>
+  </si>
+  <si>
+    <t>How machine learning enhances athlete training.</t>
+  </si>
+  <si>
+    <t>Brooks</t>
+  </si>
+  <si>
+    <t>Sports Science</t>
+  </si>
+  <si>
+    <t>Smart Traffic Management with AI</t>
+  </si>
+  <si>
+    <t>Reducing congestion with predictive AI systems.</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Next-Gen Biometric Authentication</t>
+  </si>
+  <si>
+    <t>Security advancements in facial and fingerprint recognition.</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>AI in Archaeology</t>
+  </si>
+  <si>
+    <t>Using deep learning to reconstruct ancient civilizations.</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>Anthropology &amp; AI</t>
+  </si>
+  <si>
+    <t>Deepfake Detection with AI</t>
+  </si>
+  <si>
+    <t>Preventing AI-generated misinformation.</t>
+  </si>
+  <si>
+    <t>Ward</t>
+  </si>
+  <si>
+    <t>Wireless Charging for Electric Vehicles</t>
+  </si>
+  <si>
+    <t>Improving efficiency in wireless power transfer.</t>
+  </si>
+  <si>
+    <t>Aiden</t>
+  </si>
+  <si>
+    <t>Cox</t>
+  </si>
+  <si>
+    <t>AI-Powered Chatbots for Healthcare</t>
+  </si>
+  <si>
+    <t>Virtual assistants for medical diagnosis.</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Ocean Cleanup with Robotics</t>
+  </si>
+  <si>
+    <t>Using AI-driven robots to remove ocean waste.</t>
+  </si>
+  <si>
+    <t>Flores</t>
+  </si>
+  <si>
+    <t>AI and Personalized Nutrition</t>
+  </si>
+  <si>
+    <t>Machine learning for custom diet plans.</t>
+  </si>
+  <si>
+    <t>Richardson</t>
+  </si>
+  <si>
+    <t>Health Informatics</t>
+  </si>
+  <si>
+    <t>Space Tourism: Challenges and Innovations</t>
+  </si>
+  <si>
+    <t>The feasibility of commercial space travel.</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>AI in Smart Farming</t>
+  </si>
+  <si>
+    <t>AI-powered tools for crop monitoring.</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Bennett</t>
+  </si>
+  <si>
+    <t>AI for Earthquake Prediction</t>
+  </si>
+  <si>
+    <t>Machine learning models for seismic activity analysis.</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Geophysics</t>
+  </si>
+  <si>
+    <t>The Future of Quantum Sensors</t>
+  </si>
+  <si>
+    <t>Ultra-precise measurements for navigation and science.</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Quantum Engineering</t>
+  </si>
+  <si>
+    <t>AI and Emotional Recognition</t>
+  </si>
+  <si>
+    <t>Exploring AI’s ability to detect human emotions.</t>
+  </si>
+  <si>
+    <t>Russell</t>
+  </si>
 </sst>
 </file>
 
@@ -2917,12 +3142,24 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="5"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="A50" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -2945,11 +3182,24 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="A51" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -2972,12 +3222,24 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="A52" s="1">
+        <v>51.0</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -3000,12 +3262,24 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="A53" s="1">
+        <v>52.0</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -3028,12 +3302,24 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="A54" s="1">
+        <v>53.0</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -3056,12 +3342,24 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="A55" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -3084,12 +3382,24 @@
       <c r="Z55" s="1"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+      <c r="A56" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>250</v>
+      </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
@@ -3112,12 +3422,24 @@
       <c r="Z56" s="1"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
+      <c r="A57" s="1">
+        <v>56.0</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -3140,12 +3462,24 @@
       <c r="Z57" s="1"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="A58" s="1">
+        <v>57.0</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -3168,12 +3502,24 @@
       <c r="Z58" s="1"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
+      <c r="A59" s="1">
+        <v>58.0</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>261</v>
+      </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -3196,12 +3542,24 @@
       <c r="Z59" s="1"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+      <c r="A60" s="1">
+        <v>59.0</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>213</v>
+      </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -3224,12 +3582,24 @@
       <c r="Z60" s="1"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
+      <c r="A61" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -3252,12 +3622,24 @@
       <c r="Z61" s="1"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
+      <c r="A62" s="1">
+        <v>61.0</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -3280,12 +3662,24 @@
       <c r="Z62" s="1"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
+      <c r="A63" s="1">
+        <v>62.0</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -3308,12 +3702,24 @@
       <c r="Z63" s="1"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
+      <c r="A64" s="1">
+        <v>63.0</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>278</v>
+      </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -3336,12 +3742,24 @@
       <c r="Z64" s="1"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="A65" s="1">
+        <v>64.0</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -3364,12 +3782,24 @@
       <c r="Z65" s="1"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
+      <c r="A66" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -3392,12 +3822,24 @@
       <c r="Z66" s="1"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
+      <c r="A67" s="1">
+        <v>66.0</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>289</v>
+      </c>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -3420,12 +3862,24 @@
       <c r="Z67" s="1"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
+      <c r="A68" s="1">
+        <v>67.0</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>293</v>
+      </c>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
@@ -3448,12 +3902,24 @@
       <c r="Z68" s="1"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+      <c r="A69" s="1">
+        <v>68.0</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>204</v>
+      </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
@@ -3476,7 +3942,7 @@
       <c r="Z69" s="1"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="1"/>
+      <c r="A70" s="5"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3504,7 +3970,6 @@
       <c r="Z70" s="1"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>

</xml_diff>